<commit_message>
A1#111ZUCCHETTIXX/Zucchetti_Centro_Sistema_s.p.a/JLAB/v.9 - Correzione test4
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ZUCCHETTIXX/Zucchetti_Centro_Sistema_s.p.a/JLAB/v.9/report-checklist.xlsx
+++ b/GATEWAY/A1#111ZUCCHETTIXX/Zucchetti_Centro_Sistema_s.p.a/JLAB/v.9/report-checklist.xlsx
@@ -588,15 +588,6 @@
     <t>"2.16.840.1.113883.2.9.2.80.3.1.4.4.7e70a2b00727474a5069151376e46fdc4975ff3dbee74874ca6bc2c6a16c8818.bfeb2a9975^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
   </si>
   <si>
-    <t>2023-05-05T12:09:00Z</t>
-  </si>
-  <si>
-    <t>"07fe7eaab710f01d"</t>
-  </si>
-  <si>
-    <t>"2.16.840.1.113883.2.9.2.80.3.1.4.4.122ea19a470f4fbe4ffe36685f217e69aa26679ffa7ac022b1cb97097d0fd95a.4758485892^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
-  </si>
-  <si>
     <t>2023-05-05T15:52:00Z</t>
   </si>
   <si>
@@ -863,6 +854,15 @@
   </si>
   <si>
     <t xml:space="preserve">"2.16.840.1.113883.2.9.2.80.3.1.4.4.496082e3db886d53d2db7457bb7bf999196238e8daac0051c1643090b0d4aa4a.35b2945779^^^^urn:ihe:iti:xdw:2013:workflowInstanceId" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2023-05-31T10:33:24Z</t>
+  </si>
+  <si>
+    <t>"b64a457016d0bd94"</t>
+  </si>
+  <si>
+    <t>"2.16.840.1.113883.2.9.2.80.3.1.4.4.d3056e969a183427cae275feb3b86dbe5d6548e92da68be0aa17970dd78c7e2e.290e5e0b96^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
   </si>
 </sst>
 </file>
@@ -3766,10 +3766,10 @@
   <dimension ref="A1:T4585"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="N13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="N12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="X13" sqref="X13"/>
+      <selection pane="bottomRight" activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="37" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D2" s="36"/>
       <c r="F2" s="12"/>
@@ -4180,16 +4180,16 @@
         <v>54</v>
       </c>
       <c r="F13" s="23">
-        <v>45071</v>
+        <v>45077</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>63</v>
@@ -4229,13 +4229,13 @@
         <v>45051</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>107</v>
+        <v>172</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>108</v>
+        <v>173</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>109</v>
+        <v>174</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>63</v>
@@ -4275,13 +4275,13 @@
         <v>45051</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>63</v>
@@ -4294,20 +4294,20 @@
         <v>63</v>
       </c>
       <c r="N15" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O15" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P15" s="25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="Q15" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R15" s="26"/>
       <c r="S15" s="27" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="T15" s="28" t="s">
         <v>45</v>
@@ -4333,13 +4333,13 @@
         <v>45051</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>63</v>
@@ -4352,20 +4352,20 @@
         <v>63</v>
       </c>
       <c r="N16" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O16" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P16" s="25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="Q16" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R16" s="26"/>
       <c r="S16" s="27" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="T16" s="28" t="s">
         <v>45</v>
@@ -4404,7 +4404,7 @@
       <c r="N17" s="25"/>
       <c r="O17" s="25"/>
       <c r="P17" s="25" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="Q17" s="25" t="s">
         <v>91</v>
@@ -4413,7 +4413,7 @@
         <v>63</v>
       </c>
       <c r="S17" s="27" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T17" s="28" t="s">
         <v>45</v>
@@ -4439,16 +4439,16 @@
         <v>45051</v>
       </c>
       <c r="G18" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="I18" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="H18" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>117</v>
-      </c>
       <c r="J18" s="25" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K18" s="25"/>
       <c r="L18" s="25" t="s">
@@ -4458,20 +4458,20 @@
         <v>63</v>
       </c>
       <c r="N18" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O18" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P18" s="25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="Q18" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R18" s="26"/>
       <c r="S18" s="27" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="T18" s="28" t="s">
         <v>45</v>
@@ -4497,13 +4497,13 @@
         <v>45051</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>63</v>
@@ -4516,20 +4516,20 @@
         <v>63</v>
       </c>
       <c r="N19" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O19" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P19" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="Q19" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R19" s="26"/>
       <c r="S19" s="27" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="T19" s="28" t="s">
         <v>45</v>
@@ -4555,13 +4555,13 @@
         <v>45051</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>63</v>
@@ -4574,20 +4574,20 @@
         <v>63</v>
       </c>
       <c r="N20" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O20" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P20" s="25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="Q20" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R20" s="26"/>
       <c r="S20" s="27" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="T20" s="28" t="s">
         <v>45</v>
@@ -4613,13 +4613,13 @@
         <v>45051</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>63</v>
@@ -4632,20 +4632,20 @@
         <v>63</v>
       </c>
       <c r="N21" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O21" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P21" s="25" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="Q21" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R21" s="26"/>
       <c r="S21" s="27" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="T21" s="28" t="s">
         <v>45</v>
@@ -4671,13 +4671,13 @@
         <v>45051</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="J22" s="25" t="s">
         <v>63</v>
@@ -4690,20 +4690,20 @@
         <v>63</v>
       </c>
       <c r="N22" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O22" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P22" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q22" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R22" s="26"/>
       <c r="S22" s="27" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="T22" s="28" t="s">
         <v>45</v>
@@ -4729,13 +4729,13 @@
         <v>45051</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J23" s="25" t="s">
         <v>63</v>
@@ -4748,20 +4748,20 @@
         <v>63</v>
       </c>
       <c r="N23" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O23" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P23" s="25" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="Q23" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R23" s="26"/>
       <c r="S23" s="27" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="T23" s="28" t="s">
         <v>45</v>
@@ -4787,13 +4787,13 @@
         <v>45051</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J24" s="25" t="s">
         <v>63</v>
@@ -4806,20 +4806,20 @@
         <v>63</v>
       </c>
       <c r="N24" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O24" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P24" s="25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="Q24" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R24" s="26"/>
       <c r="S24" s="27" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="T24" s="28" t="s">
         <v>45</v>
@@ -4845,13 +4845,13 @@
         <v>45051</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="J25" s="25" t="s">
         <v>63</v>
@@ -4864,20 +4864,20 @@
         <v>63</v>
       </c>
       <c r="N25" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O25" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P25" s="25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="Q25" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R25" s="26"/>
       <c r="S25" s="27" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="T25" s="28" t="s">
         <v>45</v>
@@ -4903,13 +4903,13 @@
         <v>45051</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J26" s="25" t="s">
         <v>63</v>
@@ -4922,20 +4922,20 @@
         <v>63</v>
       </c>
       <c r="N26" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O26" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P26" s="25" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Q26" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R26" s="26"/>
       <c r="S26" s="27" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="T26" s="28" t="s">
         <v>45</v>
@@ -4961,13 +4961,13 @@
         <v>45051</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J27" s="25" t="s">
         <v>63</v>
@@ -4980,20 +4980,20 @@
         <v>63</v>
       </c>
       <c r="N27" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O27" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P27" s="25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="Q27" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R27" s="26"/>
       <c r="S27" s="27" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="T27" s="28" t="s">
         <v>45</v>
@@ -5019,13 +5019,13 @@
         <v>45051</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J28" s="25" t="s">
         <v>63</v>
@@ -5038,20 +5038,20 @@
         <v>63</v>
       </c>
       <c r="N28" s="25" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O28" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P28" s="25" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="Q28" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R28" s="26"/>
       <c r="S28" s="27" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="T28" s="28" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Modificata colonna "Gestione errore" per i casi con ID [28, 36, 44, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62]
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ZUCCHETTIXX/Zucchetti_Centro_Sistema_s.p.a/JLAB/v.9/report-checklist.xlsx
+++ b/GATEWAY/A1#111ZUCCHETTIXX/Zucchetti_Centro_Sistema_s.p.a/JLAB/v.9/report-checklist.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="168">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -600,16 +600,7 @@
     <t>"333dbd07c2607110"</t>
   </si>
   <si>
-    <t>2023-05-05T14:34:00Z</t>
-  </si>
-  <si>
     <t>2023-05-05T16:01:00Z</t>
-  </si>
-  <si>
-    <t>"66b7cfb307ad6d73"</t>
-  </si>
-  <si>
-    <t>"2.16.840.1.113883.2.9.2.80.3.1.4.4.c1ecd4b995eb48e9a67b281466676acdd11e2ba185d38c59c28be6084a24e324.eadeefb2b5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
   </si>
   <si>
     <t>"2.16.840.1.113883.2.9.2.80.3.1.4.4.ba9a344f5b672df5c7b0d818a79cb5498fa03275f95ecf586676c880939a5cc1.b3a665d188^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
@@ -619,15 +610,6 @@
   </si>
   <si>
     <t>2023-05-05T15:27:00Z</t>
-  </si>
-  <si>
-    <t>2023-05-05T14:44:00Z</t>
-  </si>
-  <si>
-    <t>"625550de2bb270d3"</t>
-  </si>
-  <si>
-    <t>"2.16.840.1.113883.2.9.2.80.3.1.4.4.2a0330b0b862a5035599609f5cbc0f2f8b4374609cc7a8413e098bb6348b2c16.1c1b1912ec^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
   </si>
   <si>
     <t>2023-05-05T14:47:00Z</t>
@@ -705,40 +687,10 @@
     <t>Zucchetti Centro Sistema s.p.a</t>
   </si>
   <si>
-    <t>Sì</t>
-  </si>
-  <si>
-    <t>Si procede in backoffice all'analisi  dell'errore ricevuto</t>
-  </si>
-  <si>
-    <t>Viene restituito un report con il messaggio di errore ricevuto dal servizio di validazione e si procede all'analisi in backoffice</t>
-  </si>
-  <si>
     <t>Si è generato errore, quindi esito PASS</t>
   </si>
   <si>
     <t xml:space="preserve">Viene restituito un report con il messaggio di errore ricevuto dal servizio di validazione </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si procede lato LIS con l' inserimento del comune </t>
-  </si>
-  <si>
-    <t>Si procede lato LIS con la correzione del codice fiscale  che ha generato l'errore</t>
-  </si>
-  <si>
-    <t>Si procede lato LIS con l' inserimento del nome del paziente</t>
-  </si>
-  <si>
-    <t>Si procede lato LIS con la correzione del genere</t>
-  </si>
-  <si>
-    <t>Si procede alla correzione del codice associato all'analisi che ha generato l'errore</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Response : 400 
- Errore rilevato : Errore di sintassi. 
- Tipo errore : /msg/syntax 
- detail : ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'confidentialityCode' is not valid with respect to its type, 'cs'.                                                      Si è generato errore, quindi esito PASS</t>
   </si>
   <si>
     <t xml:space="preserve"> Response : 422 
@@ -746,13 +698,6 @@
  Tipo errore : /msg/semantic 
  detail : [ERRORE-46| codice fiscale 'prvtst01a41h501d' cittadino ed operatore: 16 cifre [A-Z0-9]{16}]
  Si è generato errore, quindi esito PASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Response : 422 
- Errore rilevato : Errore semantico. 
- Tipo errore : /msg/semantic 
- detail : [ERRORE-6| L'elemento  'confidentialityCode' di ClinicalDocument DEVE avere l'attributo @code  valorizzato con 'N' o 'V', e il suo @codeSystem  con '2.16.840.1.113883.5.25'],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Referto di laboratorio'.--&gt; ],[W003 | Si consiglia di utilizzare il sistema di codifica LOINC per la valorizzazione dell'elemento observation/code.--&gt; ],[W003 | Si consiglia di utilizzare il sistema di codifica LOINC per la valorizzazione dell'elemento observation/code.--&gt; ],[W003 | Si consiglia di utilizzare il sistema di codifica LOINC per la valorizzazione dell'elemento observation/code.--&gt; ]
-Si è generato errore, quindi esito PASS</t>
   </si>
   <si>
     <t xml:space="preserve">  Response : 422 
@@ -863,6 +808,33 @@
   </si>
   <si>
     <t>"2.16.840.1.113883.2.9.2.80.3.1.4.4.d3056e969a183427cae275feb3b86dbe5d6548e92da68be0aa17970dd78c7e2e.290e5e0b96^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
+  </si>
+  <si>
+    <t>Viene restituito un report con il messaggio di errore ricevuto dal servizio di validazione, l'operatore ha la possibilità di correggere l'errore e procedere nuovamente alla produzione e validazione del documento manualmente in back office.</t>
+  </si>
+  <si>
+    <t>Viene restituito un report con il messaggio di errore ricevuto dal servizio di validazione, l'operazione di retry viene eseguita manualmente dall’operatore in back office.</t>
+  </si>
+  <si>
+    <t>Il campo non puo' mai essere nullo.</t>
+  </si>
+  <si>
+    <t>Si procede lato LIS con la correzione del codice fiscale  che ha generato l'errore. L'operazione di retry viene eseguita manualmente dall’operatore in back office.</t>
+  </si>
+  <si>
+    <t>Si procede lato LIS con l' inserimento del comune. L'operazione di retry viene eseguita manualmente dall’operatore in back office.</t>
+  </si>
+  <si>
+    <t>Si procede lato LIS con l' inserimento del nome del paziente. L'operazione di retry viene eseguita manualmente dall’operatore in back office.</t>
+  </si>
+  <si>
+    <t>Si procede lato LIS con la correzione del genere. L'operazione di retry viene eseguita manualmente dall’operatore in back office.</t>
+  </si>
+  <si>
+    <t>Si procede in backoffice all'analisi  dell'errore ricevuto. L'operazione di retry viene eseguita manualmente dall’operatore in back office.</t>
+  </si>
+  <si>
+    <t>Si procede alla correzione del codice associato all'analisi che ha generato l'errore. L'operazione di retry viene eseguita manualmente dall’operatore in back office.</t>
   </si>
 </sst>
 </file>
@@ -3766,10 +3738,10 @@
   <dimension ref="A1:T4585"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="N12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="X14" sqref="X14"/>
+      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3813,7 +3785,7 @@
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="37" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D2" s="36"/>
       <c r="F2" s="12"/>
@@ -3944,7 +3916,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="15"/>
     </row>
-    <row r="8" spans="1:20" ht="14.25" customHeight="1">
+    <row r="8" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
@@ -4183,13 +4155,13 @@
         <v>45077</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>63</v>
@@ -4229,13 +4201,13 @@
         <v>45051</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>63</v>
@@ -4255,7 +4227,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="15" spans="1:20" ht="144.6" thickBot="1">
       <c r="A15" s="20">
         <v>28</v>
       </c>
@@ -4294,20 +4266,20 @@
         <v>63</v>
       </c>
       <c r="N15" s="25" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O15" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P15" s="25" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="Q15" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R15" s="26"/>
       <c r="S15" s="27" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="T15" s="28" t="s">
         <v>45</v>
@@ -4333,7 +4305,7 @@
         <v>45051</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H16" s="24" t="s">
         <v>110</v>
@@ -4352,26 +4324,26 @@
         <v>63</v>
       </c>
       <c r="N16" s="25" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O16" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P16" s="25" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="Q16" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R16" s="26"/>
       <c r="S16" s="27" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="T16" s="28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="58.2" thickBot="1">
+    <row r="17" spans="1:20" ht="87" thickBot="1">
       <c r="A17" s="20">
         <v>44</v>
       </c>
@@ -4404,7 +4376,7 @@
       <c r="N17" s="25"/>
       <c r="O17" s="25"/>
       <c r="P17" s="25" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="Q17" s="25" t="s">
         <v>91</v>
@@ -4413,13 +4385,13 @@
         <v>63</v>
       </c>
       <c r="S17" s="27" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="T17" s="28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="173.4" thickBot="1">
+    <row r="18" spans="1:20" ht="115.8" thickBot="1">
       <c r="A18" s="20">
         <v>52</v>
       </c>
@@ -4438,41 +4410,23 @@
       <c r="F18" s="23">
         <v>45051</v>
       </c>
-      <c r="G18" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>114</v>
-      </c>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
       <c r="J18" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="M18" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="N18" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="O18" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="P18" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q18" s="25" t="s">
-        <v>91</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="K18" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
       <c r="R18" s="26"/>
-      <c r="S18" s="27" t="s">
-        <v>156</v>
-      </c>
+      <c r="S18" s="27"/>
       <c r="T18" s="28" t="s">
         <v>45</v>
       </c>
@@ -4497,13 +4451,13 @@
         <v>45051</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>63</v>
@@ -4516,26 +4470,26 @@
         <v>63</v>
       </c>
       <c r="N19" s="25" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O19" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P19" s="25" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="Q19" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R19" s="26"/>
       <c r="S19" s="27" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="T19" s="28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="389.4" thickBot="1">
+    <row r="20" spans="1:20" ht="115.8" thickBot="1">
       <c r="A20" s="20">
         <v>54</v>
       </c>
@@ -4554,46 +4508,28 @@
       <c r="F20" s="23">
         <v>45051</v>
       </c>
-      <c r="G20" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>120</v>
-      </c>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
       <c r="J20" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="M20" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="N20" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="O20" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="P20" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q20" s="25" t="s">
-        <v>91</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="K20" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="L20" s="25"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="25"/>
+      <c r="Q20" s="25"/>
       <c r="R20" s="26"/>
-      <c r="S20" s="27" t="s">
-        <v>158</v>
-      </c>
+      <c r="S20" s="27"/>
       <c r="T20" s="28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="288.60000000000002" thickBot="1">
+    <row r="21" spans="1:20" ht="303" thickBot="1">
       <c r="A21" s="20">
         <v>55</v>
       </c>
@@ -4613,13 +4549,13 @@
         <v>45051</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>63</v>
@@ -4632,26 +4568,26 @@
         <v>63</v>
       </c>
       <c r="N21" s="25" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O21" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P21" s="25" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="Q21" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R21" s="26"/>
       <c r="S21" s="27" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="T21" s="28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="274.2" thickBot="1">
+    <row r="22" spans="1:20" ht="288.60000000000002" thickBot="1">
       <c r="A22" s="20">
         <v>56</v>
       </c>
@@ -4671,13 +4607,13 @@
         <v>45051</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J22" s="25" t="s">
         <v>63</v>
@@ -4690,26 +4626,26 @@
         <v>63</v>
       </c>
       <c r="N22" s="25" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O22" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P22" s="25" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="Q22" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R22" s="26"/>
       <c r="S22" s="27" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="T22" s="28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="130.19999999999999" thickBot="1">
+    <row r="23" spans="1:20" ht="144.6" thickBot="1">
       <c r="A23" s="20">
         <v>57</v>
       </c>
@@ -4729,13 +4665,13 @@
         <v>45051</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="J23" s="25" t="s">
         <v>63</v>
@@ -4748,20 +4684,20 @@
         <v>63</v>
       </c>
       <c r="N23" s="25" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O23" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P23" s="25" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="Q23" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R23" s="26"/>
       <c r="S23" s="27" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="T23" s="28" t="s">
         <v>45</v>
@@ -4787,13 +4723,13 @@
         <v>45051</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="J24" s="25" t="s">
         <v>63</v>
@@ -4806,20 +4742,20 @@
         <v>63</v>
       </c>
       <c r="N24" s="25" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O24" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P24" s="25" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="Q24" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R24" s="26"/>
       <c r="S24" s="27" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="T24" s="28" t="s">
         <v>45</v>
@@ -4845,13 +4781,13 @@
         <v>45051</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="J25" s="25" t="s">
         <v>63</v>
@@ -4864,20 +4800,20 @@
         <v>63</v>
       </c>
       <c r="N25" s="25" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O25" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P25" s="25" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="Q25" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R25" s="26"/>
       <c r="S25" s="27" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="T25" s="28" t="s">
         <v>45</v>
@@ -4903,13 +4839,13 @@
         <v>45051</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="J26" s="25" t="s">
         <v>63</v>
@@ -4922,20 +4858,20 @@
         <v>63</v>
       </c>
       <c r="N26" s="25" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O26" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P26" s="25" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="Q26" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R26" s="26"/>
       <c r="S26" s="27" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="T26" s="28" t="s">
         <v>45</v>
@@ -4961,13 +4897,13 @@
         <v>45051</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="J27" s="25" t="s">
         <v>63</v>
@@ -4980,20 +4916,20 @@
         <v>63</v>
       </c>
       <c r="N27" s="25" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O27" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P27" s="25" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="Q27" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R27" s="26"/>
       <c r="S27" s="27" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="T27" s="28" t="s">
         <v>45</v>
@@ -5019,13 +4955,13 @@
         <v>45051</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="J28" s="25" t="s">
         <v>63</v>
@@ -5038,20 +4974,20 @@
         <v>63</v>
       </c>
       <c r="N28" s="25" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="O28" s="25" t="s">
         <v>63</v>
       </c>
       <c r="P28" s="25" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="Q28" s="25" t="s">
         <v>91</v>
       </c>
       <c r="R28" s="26"/>
       <c r="S28" s="27" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="T28" s="28" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Correzione test con ID [52, 54]
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ZUCCHETTIXX/Zucchetti_Centro_Sistema_s.p.a/JLAB/v.9/report-checklist.xlsx
+++ b/GATEWAY/A1#111ZUCCHETTIXX/Zucchetti_Centro_Sistema_s.p.a/JLAB/v.9/report-checklist.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="176">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -816,9 +816,6 @@
     <t>Viene restituito un report con il messaggio di errore ricevuto dal servizio di validazione, l'operazione di retry viene eseguita manualmente dall’operatore in back office.</t>
   </si>
   <si>
-    <t>Il campo non puo' mai essere nullo.</t>
-  </si>
-  <si>
     <t>Si procede lato LIS con la correzione del codice fiscale  che ha generato l'errore. L'operazione di retry viene eseguita manualmente dall’operatore in back office.</t>
   </si>
   <si>
@@ -835,6 +832,40 @@
   </si>
   <si>
     <t>Si procede alla correzione del codice associato all'analisi che ha generato l'errore. L'operazione di retry viene eseguita manualmente dall’operatore in back office.</t>
+  </si>
+  <si>
+    <t>2023-05-05T14:34:00Z</t>
+  </si>
+  <si>
+    <t>66b7cfb307ad6d73</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.c1ecd4b995eb48e9a67b281466676acdd11e2ba185d38c59c28be6084a24e324.eadeefb2b5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Sì</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Response : 400 
+ Errore rilevato : Errore di sintassi. 
+ Tipo errore : /msg/syntax 
+ detail : ERROR: -1,-1 cvc-pattern-valid: Value '' is not facet-valid with respect to pattern '[^\s]+' for type 'cs'.,ERROR: -1,-1 cvc-attribute.3: The value '' of attribute 'code' on element 'confidentialityCode' is not valid with respect to its type, 'cs'.                                                      Si è generato errore, quindi esito PASS</t>
+  </si>
+  <si>
+    <t>2023-05-05T14:44:00Z</t>
+  </si>
+  <si>
+    <t>625550de2bb270d3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.2a0330b0b862a5035599609f5cbc0f2f8b4374609cc7a8413e098bb6348b2c16.1c1b1912ec^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Response : 422 
+ Errore rilevato : Errore semantico. 
+ Tipo errore : /msg/semantic 
+ detail : [ERRORE-6| L'elemento  'confidentialityCode' di ClinicalDocument DEVE avere l'attributo @code  valorizzato con 'N' o 'V', e il suo @codeSystem  con '2.16.840.1.113883.5.25'],[W001| Si raccomanda di valorizzare gli attributi dell'elemento ClinicalDocument/code nel seguente modo: @codeSystemName ='LOINC' e @displayName ='Referto di laboratorio'.--&gt; ],[W003 | Si consiglia di utilizzare il sistema di codifica LOINC per la valorizzazione dell'elemento observation/code.--&gt; ],[W003 | Si consiglia di utilizzare il sistema di codifica LOINC per la valorizzazione dell'elemento observation/code.--&gt; ],[W003 | Si consiglia di utilizzare il sistema di codifica LOINC per la valorizzazione dell'elemento observation/code.--&gt; ]
+Si è generato errore, quindi esito PASS</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1256,6 +1287,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3738,10 +3772,10 @@
   <dimension ref="A1:T4585"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="K18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
+      <selection pane="bottomRight" activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -3780,14 +3814,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="36"/>
+      <c r="D2" s="37"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3805,14 +3839,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="44" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="36"/>
+      <c r="D3" s="37"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -3830,12 +3864,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="44" t="s">
+      <c r="A4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -3854,12 +3888,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="42"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="44" t="s">
+      <c r="A5" s="43"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="37"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -3877,8 +3911,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="33"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4227,7 +4261,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="144.6" thickBot="1">
+    <row r="15" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A15" s="20">
         <v>28</v>
       </c>
@@ -4391,7 +4425,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="115.8" thickBot="1">
+    <row r="18" spans="1:20" ht="173.4" thickBot="1">
       <c r="A18" s="20">
         <v>52</v>
       </c>
@@ -4410,23 +4444,41 @@
       <c r="F18" s="23">
         <v>45051</v>
       </c>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
+      <c r="G18" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>169</v>
+      </c>
       <c r="J18" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="K18" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="25"/>
+        <v>170</v>
+      </c>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="M18" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="N18" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="O18" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="P18" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q18" s="25" t="s">
+        <v>91</v>
+      </c>
       <c r="R18" s="26"/>
-      <c r="S18" s="27"/>
+      <c r="S18" s="33" t="s">
+        <v>171</v>
+      </c>
       <c r="T18" s="28" t="s">
         <v>45</v>
       </c>
@@ -4476,7 +4528,7 @@
         <v>63</v>
       </c>
       <c r="P19" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q19" s="25" t="s">
         <v>91</v>
@@ -4489,7 +4541,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="115.8" thickBot="1">
+    <row r="20" spans="1:20" ht="403.8" thickBot="1">
       <c r="A20" s="20">
         <v>54</v>
       </c>
@@ -4508,23 +4560,41 @@
       <c r="F20" s="23">
         <v>45051</v>
       </c>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
+      <c r="G20" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>174</v>
+      </c>
       <c r="J20" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="K20" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="25"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="25"/>
+        <v>63</v>
+      </c>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="M20" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="N20" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="O20" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="P20" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q20" s="25" t="s">
+        <v>91</v>
+      </c>
       <c r="R20" s="26"/>
-      <c r="S20" s="27"/>
+      <c r="S20" s="33" t="s">
+        <v>175</v>
+      </c>
       <c r="T20" s="28" t="s">
         <v>45</v>
       </c>
@@ -4574,7 +4644,7 @@
         <v>63</v>
       </c>
       <c r="P21" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q21" s="25" t="s">
         <v>91</v>
@@ -4587,7 +4657,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="288.60000000000002" thickBot="1">
+    <row r="22" spans="1:20" ht="274.2" thickBot="1">
       <c r="A22" s="20">
         <v>56</v>
       </c>
@@ -4632,7 +4702,7 @@
         <v>63</v>
       </c>
       <c r="P22" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q22" s="25" t="s">
         <v>91</v>
@@ -4645,7 +4715,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="144.6" thickBot="1">
+    <row r="23" spans="1:20" ht="130.19999999999999" thickBot="1">
       <c r="A23" s="20">
         <v>57</v>
       </c>
@@ -4690,7 +4760,7 @@
         <v>63</v>
       </c>
       <c r="P23" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q23" s="25" t="s">
         <v>91</v>
@@ -4748,7 +4818,7 @@
         <v>63</v>
       </c>
       <c r="P24" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q24" s="25" t="s">
         <v>91</v>
@@ -4806,7 +4876,7 @@
         <v>63</v>
       </c>
       <c r="P25" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q25" s="25" t="s">
         <v>91</v>
@@ -4864,7 +4934,7 @@
         <v>63</v>
       </c>
       <c r="P26" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q26" s="25" t="s">
         <v>91</v>
@@ -4922,7 +4992,7 @@
         <v>63</v>
       </c>
       <c r="P27" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q27" s="25" t="s">
         <v>91</v>
@@ -4980,7 +5050,7 @@
         <v>63</v>
       </c>
       <c r="P28" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q28" s="25" t="s">
         <v>91</v>

</xml_diff>